<commit_message>
added test cases for APE
</commit_message>
<xml_diff>
--- a/Tests/integrationTests/06_APE/Test_cases_APE.xlsx
+++ b/Tests/integrationTests/06_APE/Test_cases_APE.xlsx
@@ -108,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="72">
   <si>
     <t>Number</t>
   </si>
@@ -182,16 +182,6 @@
     <t>Asterics_ TestCase_11</t>
   </si>
   <si>
-    <t>Tests for 
-APE-copy tool mit APE.models, APE.projectDir und APE.buildDir
-defProjectDir
-*) Copy model to custom/bin/ARE/models
-*) Copy custom services to custom/bin/ARE/profile
-ant APE-copy
-ant deploy ohne java embedded
-ant deploy mit java embedded</t>
-  </si>
-  <si>
     <t>Applicable OS (Skip otherwise)</t>
   </si>
   <si>
@@ -204,13 +194,152 @@
     <t>APE-copy providing models file</t>
   </si>
   <si>
-    <t>Installed Asterics
-Tool: APE-copy.bat (APE-copy.sh)</t>
+    <t xml:space="preserve">1. Open terminal in APE directory and enter :
+APE-copy.bat -DAPE.models=../ARE/models/ImageDemo.acs
+2. Go to APE.buildDir (defProjectDir\build\merged\bin\ARE) and execute
+start.bat
+</t>
+  </si>
+  <si>
+    <t>JDK 8 (java and javac in PATH)
+APE/APE-copy.bat (APE-copy.sh)
+ARE/start.bat (start.sh)
+Terminal (cmd.exe, xterm,…)</t>
+  </si>
+  <si>
+    <t>1. a) The resources/plugins needed to execute ImageDemo.acs are copied to APE.buildDir: defProjectDir\build\merged\bin\ARE
+b) No messages starting with WARNING or SEVERE are printed to the console.
+Copying must succeed with:
+INFO: FINISHED copying ARE:…
+c) APE.buildDir must contain 23 .jar files
+d) APE.buildDir/LICENSE folder must contain 59 license files (.txt)
+2. The ARE must automatically deploy and start ImageDemo.acs without error message</t>
+  </si>
+  <si>
+    <t>APE-copy providing models file and project directory</t>
+  </si>
+  <si>
+    <t>APE-copy providing models file and build directory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open terminal in APE directory and enter :
+APE-copy.bat -DAPE.models=../ARE/models/ImageDemo.acs -DAPE.projectDir=APE-test
+2. Go to APE.buildDir (APE-test\build\merged\bin\ARE) and execute
+start.bat
+</t>
+  </si>
+  <si>
+    <t>1. a) A subdirectory 'APE-test' must be created and contains a copy of the 'template' folder
+a) The resources/plugins needed to execute ImageDemo.acs are copied to APE.buildDir: APE-test\build\merged\bin\ARE
+b) No messages starting with WARNING or SEVERE are printed to the console.
+Copying must succeed with:
+INFO: FINISHED copying ARE:…
+c) APE.buildDir must contain 23 .jar files
+d) APE.buildDir/LICENSE folder must contain 59 license files (.txt)
+2. The ARE must automatically deploy and start ImageDemo.acs without error message</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open terminal in APE directory and enter :
+APE-copy.bat -DAPE.models=../ARE/models/ImageDemo.acs -DAPE.buildDir=C:\Windows\Temp (/tmp on Linux, Mac)
+2. Go to the respective APE.buildDir e.g. C:\Windows\Temp\build\merged\bin\ARE and execute
+start.bat
+</t>
+  </si>
+  <si>
+    <t>1. a) The resources/plugins needed to execute ImageDemo.acs are copied to APE.buildDir: C:\Windows\Temp\build\merged\bin\ARE
+b) No messages starting with WARNING or SEVERE are printed to the console.
+Copying must succeed with:
+INFO: FINISHED copying ARE:…
+c) APE.buildDir must contain 23 .jar files
+d) APE.buildDir/LICENSE folder must contain 59 license files (.txt)
+2. The ARE must automatically deploy and start ImageDemo.acs without error message</t>
+  </si>
+  <si>
+    <t>ant APE-copy providing models file</t>
+  </si>
+  <si>
+    <t>ant APE-copy providing models file and custom services.ini files</t>
+  </si>
+  <si>
+    <t>JDK 8 (java and javac in PATH)
+ant (ant executable in PATH)
+APE/defProjectDir/build.xml
+ARE/start.bat (start.sh)
+Terminal (cmd.exe, xterm,…)
+webcam (or USB cam)</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Freshly installed OS without Java, .NET and Visual Studio 2010 preinstalled
-Provided APE included in Asterics Installer, or latest release candidate https://github.com/asterics/AsTeRICS/releases
+      <t xml:space="preserve">JDK 8 (java and javac in PATH)
+ant (ant executable in PATH)
+APE/defProjectDir/build.xml
+Terminal (cmd.exe, xterm,…)
+webcam (or USB cam)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Windows: InnoSetup &gt;= 5</t>
+    </r>
+  </si>
+  <si>
+    <t>Win</t>
+  </si>
+  <si>
+    <t>Linux</t>
+  </si>
+  <si>
+    <t>Creating native installer for windows with 
+ant deploy 
+providing models file, Java not embedded</t>
+  </si>
+  <si>
+    <t>Creating native installer for windows with 
+ant deploy 
+providing models file, Java embedded</t>
+  </si>
+  <si>
+    <t>Creating native installer for Linux with 
+ant deploy 
+providing models file, Java not embedded</t>
+  </si>
+  <si>
+    <t>Creating native installer for Linux with 
+ant deploy 
+providing models file, Java embedded</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Freshly installed OS (Win7, Ubuntu and Mac OSX) without Java, .NET and Visual Studio 2010 preinstalled
+Provided cross-platform .tar.gz with ARE and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>APE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> from https://github.com/asterics/AsTeRICS/releases
 For some tests, external dependencies exist:
 </t>
     </r>
@@ -223,7 +352,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Java Development Kit 8</t>
+      <t>Java Development Kit 8, 32-bit</t>
     </r>
     <r>
       <rPr>
@@ -279,6 +408,219 @@
       </rPr>
       <t>, for windows.exe installer: http://www.jrsoftware.org/isdl.php</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Ubuntu Linux
+JDK 8 (java and javac in PATH)
+ant (ant executable in PATH)
+APE/defProjectDir/build.xml
+Terminal (cmd.exe, xterm,…)
+webcam (or USB cam)
+</t>
+  </si>
+  <si>
+    <t>Ubuntu Linux
+JDK 8 (java and javac in PATH)
+ant (ant executable in PATH)
+APE/defProjectDir/build.xml
+Terminal (cmd.exe, xterm,…)
+webcam (or USB cam)</t>
+  </si>
+  <si>
+    <t>Creating native installer for Mac OSX with 
+ant deploy 
+providing models file, Java not embedded</t>
+  </si>
+  <si>
+    <t>Creating native installer for Mac OS X with 
+ant deploy 
+providing models file, Java embedded</t>
+  </si>
+  <si>
+    <t>Mac OSX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mac OSX
+JDK 8 (java and javac in PATH)
+ant (ant executable in PATH)
+APE/defProjectDir/build.xml
+Terminal (cmd.exe, xterm,…)
+webcam (or USB cam)
+</t>
+  </si>
+  <si>
+    <t>Mac OSX
+JDK 8 (java and javac in PATH)
+ant (ant executable in PATH)
+APE/defProjectDir/build.xml
+Terminal (cmd.exe, xterm,…)
+webcam (or USB cam)</t>
+  </si>
+  <si>
+    <t>4. ape-test-app must be installed successfully (with entry in menu, desktop)
+ape-test-app must be launchable from Start menu (Applications/Other) or desktop
+The XFaceTrackerMouse.acs must be deployed and started automatically and the mouse cursor must move according to head movements.</t>
+  </si>
+  <si>
+    <t>3. ape-test-app must be installed successfully (with entry in menu, desktop)
+ape-test-app must be launchable from Start menu or desktop
+The XFaceTrackerMouse.acs must be deployed and started automatically and the mouse cursor must move according to head movements</t>
+  </si>
+  <si>
+    <t>3. ape-test-app must be installed successfully
+ape-test-app must be launchable through
+/opt/ape-test-app/app/start.sh
+The XFaceTrackerMouse.acs must be deployed and started automatically and the mouse cursor must move according to head movements.</t>
+  </si>
+  <si>
+    <t>4. APE-test-app must be installed successfully (with entry in menu, desktop and windows 'program add or remove' panel)
+APE-test-app must be launchable from Start menu or desktop
+The XFaceTrackerMouse.acs must be deployed and started automatically and the mouse cursor must move according to head movements.</t>
+  </si>
+  <si>
+    <t>3. ape-test-app must be installed successfully (with entry in menu, desktop and windows 'program add or remove' panel)
+ape-test-app must be launchable from Start menu or desktop
+The XFaceTrackerMouse.acs must be deployed and started automatically and the mouse cursor must move according to head movements.</t>
+  </si>
+  <si>
+    <t>1. a) The resources/plugins needed to execute XFaceTrackerMouse.acs are copied to APE.buildDir: defProjectDir\build\merged\bin\ARE
+b) No messages starting with WARNING or SEVERE are printed to the console.
+Copying must succeed with:
+INFO: FINISHED copying ARE:…
+c) APE.buildDir must contain 24 .jar files
+d) APE.buildDir/LICENSE folder must contain 33 license files (.txt)
+3. The ARE must automatically deploy and start XFaceTrackerMouse.acs without error message. The camera must be opened and the mouse cursor must move according to head movements</t>
+  </si>
+  <si>
+    <t>1. Copy ../ARE/models/XFaceTrackerMouse.acs defProjectDir/custom/bin/ARE/models
+2. Open terminal in APE/defProjectDir directory and enter :
+ant APE-copy
+3. Go to APE.buildDir (defProjectDir\build\merged\bin\ARE) and execute
+start.bat</t>
+  </si>
+  <si>
+    <t>1. a) The resources/plugins needed to execute XFaceTrackerMouse.acs are copied to APE.buildDir: defProjectDir\build\merged\bin\ARE
+b) No messages starting with WARNING or SEVERE are printed to the console.
+Copying must succeed with:
+INFO: FINISHED copying ARE:…
+c) APE.buildDir must contain 25 .jar files
+d) APE.buildDir/LICENSE folder must contain 63 license files (.txt)
+3. The ARE must automatically deploy and start XFaceTrackerMouse.acs without error message. The camera must be opened and the mouse cursor must move according to head movements</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Important hint for ARE:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Press F7 to stop a running model</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (this handy to stop camera mouse models)</t>
+    </r>
+  </si>
+  <si>
+    <t>JDK 8 (java and javac in PATH)
+ant (ant executable in PATH)
+APE/defProjectDir/build.xml
+ARE/start.bat (start.sh)
+Terminal (cmd.exe, xterm,…)
+webcam (or USB cam)
+services-*ini from test cases folder</t>
+  </si>
+  <si>
+    <t>1. 
+Copy ../ARE/models/XFaceTrackerMouse.acs defProjectDir/custom/bin/ARE/models
+Copy services-*.ini to defProjectDir/custom/bin/ARE/profile folder
+2. Open terminal in APE/defProjectDir directory and enter :
+ant APE-copy
+3. Go to APE.buildDir (defProjectDir\build\merged\bin\ARE) and execute
+start.bat</t>
+  </si>
+  <si>
+    <t>1. 
+Copy ../ARE/models/XFaceTrackerMouse.acs defProjectDir/custom/bin/ARE/models
+Delete services-*.ini of defProjectDir/custom/bin/ARE/profile folder
+Copy APE.properties file to defProjectDir 
+2. Open terminal in APE/defProjectDir directory and enter :
+ant deploy
+3. Start and install 
+build\deploy\bundles\ape-test-app-0.1.exe</t>
+  </si>
+  <si>
+    <t>1. 
+Copy ../ARE/models/XFaceTrackerMouse.acs defProjectDir/custom/bin/ARE/models
+Delete services*.ini of defProjectDir/custom/bin/ARE/profile folder
+Edit defProjectDir/APE.properties, uncomment APE.embedJava and set it to
+APE.embedJava=true
+2. Open terminal in APE/defProjectDir directory and enter :
+ant deploy
+3. Deinstall Java Runtime Environments (java.exe must not existent on system)
+4. Start and install 
+build\deploy\bundles\ape-test-app-javaembedded-0.1.exe</t>
+  </si>
+  <si>
+    <t>1. 
+Copy ../ARE/models/XFaceTrackerMouse.acs defProjectDir/custom/bin/ARE/models
+Delete services-*.ini of defProjectDir/custom/bin/ARE/profile folder
+Copy APE.properties file to defProjectDir 
+2. Open terminal in APE/defProjectDir directory and enter :
+ant deploy
+3. Start and install 
+build/deploy/bundles/ape-test-app-0.1.deb with
+sudo dpkg -i build/deploy/bundles/ape-test-app-0.1.deb</t>
+  </si>
+  <si>
+    <t>1. 
+Copy ../ARE/models/XFaceTrackerMouse.acs defProjectDir/custom/bin/ARE/models
+Delete services-*.ini of defProjectDir/custom/bin/ARE/profile folder
+Edit defProjectDir/APE.properties, uncomment APE.embedJava and set it to
+APE.embedJava=true
+2. Open terminal in APE/defProjectDir directory and enter :
+ant deploy
+3. Deinstall Java Runtime Environments (java must not be  existent on system)
+4. Start and install 
+build/deploy/bundles/ape-test-app-javaembedded-0.1.deb with
+sudo dpkg -i build/deploy/bundles/ape-test-app-javaembedded-0.1.deb</t>
+  </si>
+  <si>
+    <t>1. 
+Copy ../ARE/models/XFaceTrackerMouse.acs defProjectDir/custom/bin/ARE/models
+Delete services-*.ini of defProjectDir/custom/bin/ARE/profile folder
+Copy APE.properties file to defProjectDir 
+2. Open terminal in APE/defProjectDir directory and enter :
+ant deploy
+3. Start and install 
+build/deploy/bundles/ape-test-app-0.1.dmg with
+a double click onto the file</t>
+  </si>
+  <si>
+    <t>1. 
+Copy ../ARE/models/XFaceTrackerMouse.acs defProjectDir/custom/bin/ARE/models
+Delete services-*.ini of defProjectDir/custom/bin/ARE/profile folder
+Edit defProjectDir/APE.properties, uncomment APE.embedJava and set it to
+APE.embedJava=true
+2. Open terminal in APE/defProjectDir directory and enter :
+ant deploy
+3. Deinstall Java Runtime Environments (java must not be  existent on system)
+4. Start and install 
+build/deploy/bundles/ape-test-app-javaembedded-0.1.dmg with
+a double click onto the file</t>
   </si>
 </sst>
 </file>
@@ -669,7 +1011,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -679,16 +1021,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.7109375" customWidth="1"/>
     <col min="2" max="3" width="42" customWidth="1"/>
-    <col min="4" max="4" width="49.28515625" customWidth="1"/>
-    <col min="5" max="5" width="48.28515625" customWidth="1"/>
+    <col min="4" max="4" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="55" customWidth="1"/>
     <col min="6" max="6" width="36.42578125" customWidth="1"/>
     <col min="7" max="7" width="68.28515625" customWidth="1"/>
   </cols>
@@ -709,30 +1051,30 @@
         <v>7</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>11</v>
       </c>
       <c r="F2" s="7"/>
     </row>
-    <row r="3" spans="1:7" ht="272.25" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" ht="287.25" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="152.25" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" ht="47.25" x14ac:dyDescent="0.4">
       <c r="A4" s="1"/>
-      <c r="B4" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="8"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -742,7 +1084,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>2</v>
@@ -757,159 +1099,241 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="285.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
+      <c r="E7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="G7" s="5"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="300" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="5"/>
+      <c r="B8" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="C8" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
+        <v>25</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="303.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="5"/>
+      <c r="B9" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="C9" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
+        <v>25</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="1:7" ht="77.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="345.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="5"/>
+      <c r="B10" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="C10" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
+        <v>25</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>62</v>
+      </c>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" spans="1:7" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="336.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="5"/>
+      <c r="B11" s="5" t="s">
+        <v>38</v>
+      </c>
       <c r="C11" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
+        <v>25</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>60</v>
+      </c>
       <c r="G11" s="5"/>
     </row>
-    <row r="12" spans="1:7" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="335.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="5"/>
+      <c r="B12" s="5" t="s">
+        <v>43</v>
+      </c>
       <c r="C12" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
+        <v>41</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="G12" s="5"/>
     </row>
-    <row r="13" spans="1:7" ht="101.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="305.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="5"/>
+      <c r="B13" s="5" t="s">
+        <v>44</v>
+      </c>
       <c r="C13" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
+        <v>41</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>58</v>
+      </c>
       <c r="G13" s="5"/>
     </row>
-    <row r="14" spans="1:7" ht="140.44999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="285" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="5"/>
+      <c r="B14" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="C14" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
+        <v>42</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>57</v>
+      </c>
       <c r="G14" s="5"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="315" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="5"/>
+      <c r="B15" s="5" t="s">
+        <v>46</v>
+      </c>
       <c r="C15" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
+        <v>42</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>55</v>
+      </c>
       <c r="G15" s="5"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="210" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="5"/>
+      <c r="B16" s="5" t="s">
+        <v>50</v>
+      </c>
       <c r="C16" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
+        <v>52</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>56</v>
+      </c>
       <c r="G16" s="5"/>
     </row>
-    <row r="17" spans="1:7" ht="122.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="346.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="5"/>
+      <c r="B17" s="5" t="s">
+        <v>51</v>
+      </c>
       <c r="C17" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
+        <v>52</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>55</v>
+      </c>
       <c r="G17" s="5"/>
     </row>
     <row r="18" spans="1:7" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
-      <c r="C18" s="5" t="s">
-        <v>26</v>
-      </c>
+      <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>

</xml_diff>